<commit_message>
Update AI framework version 1.0 build 2024.11.28.
</commit_message>
<xml_diff>
--- a/4_testing/ava/2024.01.22/TestResult-Orbit-100x64-Test0.25-2024.01.26.xlsx
+++ b/4_testing/ava/2024.01.22/TestResult-Orbit-100x64-Test0.25-2024.01.26.xlsx
@@ -327,16 +327,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.2064</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.23330000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2.7900000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,16 +398,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.2064</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.2334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.16039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2.7699999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,16 +469,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.1221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.9300000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>7.0400000000000004E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -540,16 +540,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.1229</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.9699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>7.0199999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -611,16 +611,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.2064</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.2334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2.7900000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,16 +682,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.12180000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.8899999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>7.1400000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -755,16 +755,16 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.20669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.2336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.161</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2.7900000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,7 +1863,7 @@
   <dimension ref="A2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H21"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1900,229 +1900,495 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="B3" s="2">
+        <v>0.23019999999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3.8899999999999997E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.23019999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="B4" s="2">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.2286</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.82E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.9099999999999998E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.2296</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.2296</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="B5" s="2">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.22839999999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.2306</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.82E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.2298</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="B6" s="2">
+        <v>0.23080000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.67E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.23219999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="2">
+        <v>0.2316</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.23119999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.41E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.23180000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.2326</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="B8" s="2">
+        <v>0.23280000000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.23269999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.7899999999999998E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.23219999999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.2326</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="B9" s="2">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.23280000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.99E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.23269999999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.2336</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="B10" s="2">
+        <v>0.23330000000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.2334</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.1400000000000003E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.2334</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.2334</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="B11" s="2">
+        <v>0.23019999999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.23069999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.2298</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7.8799999999999995E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.22969999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="B12" s="2">
+        <v>0.1923</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.19520000000000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.14380000000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.1452</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.14649999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.1923</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="B13" s="2">
+        <v>0.18279999999999999</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.183</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.182</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.1542</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.18149999999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.1736</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.1721</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16450000000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.1641</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.17069999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="B15" s="2">
+        <v>0.16220000000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.16389999999999999</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.17269999999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.17369999999999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.16309999999999999</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.16259999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="B16" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.16039999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.1825</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.1827</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.184</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.161</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="B17" s="2">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.19159999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.193</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.16350000000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.19239999999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.1678</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="B18" s="2">
+        <v>0.17929999999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.1807</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.20069999999999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.20080000000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.20069999999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.18240000000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="2">
+        <v>0.1963</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.19670000000000001</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.20780000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.20780000000000001</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.1968</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.2079</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.1993</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="2">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.2104</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.2127</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.21260000000000001</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.2097</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.2127</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.21060000000000001</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="2">
+        <v>0.21609999999999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.21609999999999999</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.216</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.21609999999999999</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
@@ -2151,37 +2417,37 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="e">
+      <c r="B24" s="1">
         <f>ROUND(AVERAGE(B3:B21),4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" s="1" t="e">
+        <v>0.2064</v>
+      </c>
+      <c r="C24" s="1">
         <f t="shared" ref="C24:G24" si="0">ROUND(AVERAGE(C3:C21),4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D24" s="1" t="e">
+        <v>0.2064</v>
+      </c>
+      <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="1" t="e">
+        <v>0.1221</v>
+      </c>
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F24" s="1" t="e">
+        <v>0.1229</v>
+      </c>
+      <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G24" s="1" t="e">
+        <v>0.2064</v>
+      </c>
+      <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="1" t="e">
+        <v>0.12180000000000001</v>
+      </c>
+      <c r="H24" s="1">
         <f t="shared" ref="H24" si="1">ROUND(AVERAGE(H3:H21),4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" s="3" t="e">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="I24" s="3">
         <f>MAX(B24:H24)</f>
-        <v>#DIV/0!</v>
+        <v>0.20669999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -2190,35 +2456,35 @@
       </c>
       <c r="B25" s="2">
         <f t="shared" ref="B25:H25" si="2">ROUND(MAX(B2:B21),4)</f>
-        <v>0</v>
+        <v>0.23330000000000001</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2334</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.21560000000000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.21560000000000001</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2334</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.21560000000000001</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2336</v>
       </c>
       <c r="I25" s="4">
         <f>MAX(B25:H25)</f>
-        <v>0</v>
+        <v>0.2336</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2227,72 +2493,72 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" ref="B26:H26" si="3">ROUND(MIN(B3:B21),4)</f>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16039999999999999</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.9300000000000002E-2</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.9699999999999999E-2</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.8899999999999997E-2</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.161</v>
       </c>
       <c r="I26" s="4">
         <f>MIN(B26:H26)</f>
-        <v>0</v>
+        <v>3.8899999999999997E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="e">
+      <c r="B27" s="1">
         <f t="shared" ref="B27:G27" si="4">ROUND(_xlfn.STDEV.S(B3:B21),4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C27" s="1" t="e">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="C27" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D27" s="1" t="e">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="D27" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="1" t="e">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="E27" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="1" t="e">
+        <v>7.0199999999999999E-2</v>
+      </c>
+      <c r="F27" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="1" t="e">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="G27" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H27" s="1" t="e">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="H27" s="1">
         <f t="shared" ref="H27" si="5">ROUND(_xlfn.STDEV.S(H3:H21),4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" s="3" t="e">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="I27" s="3">
         <f>MIN(B27:H27)</f>
-        <v>#DIV/0!</v>
+        <v>2.7699999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>